<commit_message>
FFM FUNCIONAL CON TENSORFLOW
</commit_message>
<xml_diff>
--- a/data/Perceptron.xlsx
+++ b/data/Perceptron.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\EIA\Decimo\Sistemas Inteligentes\SI_2023_2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61294ED-498B-44EE-A590-FBCB85D2E8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1AB80E-B935-4715-8649-141B6BDD67A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CA813501-0022-4F32-9A45-E7F1ABEDB5C1}"/>
+    <workbookView xWindow="2810" yWindow="1360" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{CA813501-0022-4F32-9A45-E7F1ABEDB5C1}"/>
   </bookViews>
   <sheets>
     <sheet name="ORMANUAL" sheetId="1" r:id="rId1"/>
     <sheet name="ANDTABLA" sheetId="4" r:id="rId2"/>
-    <sheet name="ORTABLA" sheetId="2" r:id="rId3"/>
+    <sheet name="XORTABLA" sheetId="2" r:id="rId3"/>
     <sheet name="EJERCICIO" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -2468,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB73D9CD-A483-4E62-9EA9-F994F32833CF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2538,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1D94F7-5BFE-4FF4-826E-8245F831A8DD}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>